<commit_message>
update wireframes + add ideas
</commit_message>
<xml_diff>
--- a/docs/Sitemap/sitemap.xlsx
+++ b/docs/Sitemap/sitemap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamd\Documents\HOSPI_WEBSITE\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamd\code\Hospitalia_website\docs\Sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3682341F-5750-41E5-A797-D8BC3BDB4255}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1202106D-5FFF-4ACC-934E-1C18AB7CB63A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{664A07AB-C806-401B-83CE-6E08CA2DDF90}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>HOME</t>
   </si>
   <si>
-    <t>PRAESIDIUM</t>
-  </si>
-  <si>
     <t>HOSPITALIA</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>HUIDIG PREASIDIUM</t>
   </si>
   <si>
-    <t>PRO-PRAESIDIA</t>
-  </si>
-  <si>
     <t>INFO</t>
   </si>
   <si>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>SITE MAP</t>
+  </si>
+  <si>
+    <t>PREASIDIUM</t>
+  </si>
+  <si>
+    <t>PRO-PREASIDIA</t>
   </si>
 </sst>
 </file>
@@ -222,6 +222,29 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,29 +256,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,7 +574,7 @@
   <dimension ref="B1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:V19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,198 +584,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
+      <c r="B1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="C3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C4" s="12"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
     </row>
     <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="L5" s="7"/>
-      <c r="O5" s="8"/>
-      <c r="Q5" s="10"/>
-      <c r="T5" s="10"/>
-    </row>
-    <row r="6" spans="2:24" s="15" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="C5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="L5" s="3"/>
+      <c r="O5" s="4"/>
+      <c r="Q5" s="6"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="2:24" s="9" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="E6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="11"/>
+      <c r="H6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="11"/>
+      <c r="K6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="K6" s="13" t="s">
+      <c r="L6" s="11"/>
+      <c r="N6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="N6" s="13" t="s">
+      <c r="O6" s="11"/>
+      <c r="Q6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="11"/>
+      <c r="T6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="14"/>
-      <c r="Q6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="14"/>
-      <c r="T6" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="17"/>
-    </row>
-    <row r="7" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="16"/>
+      <c r="E8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="16"/>
+      <c r="H8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="K8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="E10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="H10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="K10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="16"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="5"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+    </row>
+    <row r="12" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="H8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="K8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="E10" s="2" t="s">
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="K10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-    </row>
-    <row r="11" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="9"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-    </row>
-    <row r="12" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="2" t="s">
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="2" t="s">
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:O3"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="B1:U1"/>
@@ -792,15 +801,6 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>